<commit_message>
Test on MoNu dataset
</commit_message>
<xml_diff>
--- a/Models/Metrics.xlsx
+++ b/Models/Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\Desktop\Università\Tesi magistrale\FedMix\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343406B8-88C5-462B-A386-FB314FBCAC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9372DBA3-BBD3-49F6-9EC8-D377CD5A635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12315" yWindow="1650" windowWidth="14925" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Accuracy</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Jaccard Index</t>
+  </si>
+  <si>
+    <t>Fed on MoNu</t>
+  </si>
+  <si>
+    <t>FedAvg (External Test Data)</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,507 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -629,15 +1135,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:J9"/>
+  <dimension ref="D4:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
@@ -666,7 +1172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="4:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
@@ -689,7 +1195,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="7" spans="4:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
@@ -712,7 +1218,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="8" spans="4:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
@@ -758,38 +1264,110 @@
         <v>0.65900000000000003</v>
       </c>
     </row>
+    <row r="10" spans="4:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="4:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.873</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.63200000000000001</v>
+      </c>
+    </row>
+    <row r="18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="E6:E9">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="E6:E9 E13">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F9">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="F6:F9 F13 I6:I9 I13">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G9">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="G6:G9 G13">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="greaterThan">
+      <formula>0.8115</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="greaterThan">
       <formula>0.85</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>0.8115</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H9">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="H6:H9 H13">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="lessThan">
       <formula>0.195</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6:I9">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
-      <formula>0.8</formula>
+  <conditionalFormatting sqref="J6:J9 J13">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+      <formula>0.68</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:J9">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
-      <formula>0.68</formula>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>0.891</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0.6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>0.22</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>0.227</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0.77</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0.63</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
3 Clients FedAvg Results
</commit_message>
<xml_diff>
--- a/Models/Metrics.xlsx
+++ b/Models/Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\Desktop\Università\Tesi magistrale\FedMix\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC9773A-2B20-4256-9C4C-8B1A2C4570FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4D4C8E-0B23-48C7-B849-EB84B241D6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9270" yWindow="3300" windowWidth="16980" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="25">
   <si>
     <t>Accuracy</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>FedRGD (External Test Data)</t>
+  </si>
+  <si>
+    <t>FedAvg (3 Clients)</t>
+  </si>
+  <si>
+    <t>MoNu</t>
   </si>
 </sst>
 </file>
@@ -263,7 +269,17 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="394">
+  <dxfs count="737">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -566,6 +582,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -956,6 +982,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1186,6 +1222,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1356,6 +1412,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1746,6 +1812,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1966,6 +2042,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2136,6 +2232,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2526,6 +2632,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2746,6 +2862,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2916,6 +3052,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3526,6 +3672,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3696,6 +3872,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -4101,6 +4287,3256 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4480,10 +7916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:AT19"/>
+  <dimension ref="D4:BC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13:P15"/>
+    <sheetView tabSelected="1" topLeftCell="AS4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC6" sqref="BC6:BC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4500,10 +7936,12 @@
     <col min="32" max="37" width="13.7109375" customWidth="1"/>
     <col min="40" max="40" width="28.42578125" customWidth="1"/>
     <col min="41" max="46" width="13.85546875" customWidth="1"/>
+    <col min="49" max="49" width="28.140625" customWidth="1"/>
+    <col min="50" max="55" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:46" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:55" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
@@ -4609,8 +8047,29 @@
       <c r="AT5" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="AW5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC5" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
@@ -4716,8 +8175,29 @@
       <c r="AT6" s="7">
         <v>0.191</v>
       </c>
+      <c r="AW6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX6" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="AY6" s="7">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="AZ6" s="7">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="BA6" s="7">
+        <v>0.221</v>
+      </c>
+      <c r="BB6" s="7">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="BC6" s="7">
+        <v>0.64900000000000002</v>
+      </c>
     </row>
-    <row r="7" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4823,8 +8303,29 @@
       <c r="AT7" s="7">
         <v>7.3999999999999996E-2</v>
       </c>
+      <c r="AW7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX7" s="7">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY7" s="7">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="AZ7" s="7">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="BA7" s="7">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="BB7" s="7">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="BC7" s="7">
+        <v>0.40600000000000003</v>
+      </c>
     </row>
-    <row r="8" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
@@ -4909,8 +8410,29 @@
       <c r="AT8" s="7">
         <v>0.191</v>
       </c>
+      <c r="AW8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX8" s="7">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="AY8" s="7">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="AZ8" s="7">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="BA8" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="BB8" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="BC8" s="7">
+        <v>0.55600000000000005</v>
+      </c>
     </row>
-    <row r="9" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
@@ -4995,9 +8517,75 @@
       <c r="AT9" s="7">
         <v>7.3999999999999996E-2</v>
       </c>
+      <c r="AW9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AX9" s="7">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="AY9" s="7">
+        <v>0.81</v>
+      </c>
+      <c r="AZ9" s="7">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="BA9" s="7">
+        <v>0.186</v>
+      </c>
+      <c r="BB9" s="7">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="BC9" s="7">
+        <v>0.69099999999999995</v>
+      </c>
     </row>
-    <row r="10" spans="4:46" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AW10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX10" s="7">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="AY10" s="7">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="AZ10" s="7">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="BA10" s="7">
+        <v>0.214</v>
+      </c>
+      <c r="BB10" s="7">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="BC10" s="7">
+        <v>0.65700000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AW11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX11" s="7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AY11" s="7">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="AZ11" s="7">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="BA11" s="7">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="BB11" s="7">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="BC11" s="7">
+        <v>0.53800000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
@@ -5104,7 +8692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
@@ -5211,7 +8799,7 @@
         <v>0.216</v>
       </c>
     </row>
-    <row r="14" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
@@ -5318,7 +8906,7 @@
         <v>0.216</v>
       </c>
     </row>
-    <row r="15" spans="4:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
@@ -5407,380 +8995,400 @@
     <row r="18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="E6:E9 E13:E15">
-    <cfRule type="cellIs" dxfId="158" priority="105" operator="greaterThan">
+  <conditionalFormatting sqref="E6:E9 E13:E15 AX6:AX11">
+    <cfRule type="cellIs" dxfId="166" priority="118" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="cellIs" dxfId="157" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="165" priority="76" operator="greaterThan">
       <formula>0.884</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="164" priority="77" operator="greaterThan">
       <formula>0.893</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="155" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="163" priority="111" operator="greaterThan">
       <formula>0.898</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F9 I6:I9 F13:F15 I13:I15">
-    <cfRule type="cellIs" dxfId="154" priority="104" operator="greaterThan">
+  <conditionalFormatting sqref="F6:F9 I6:I9 F13:F15 I13:I15 AY6:AY11 BB6:BB11">
+    <cfRule type="cellIs" dxfId="162" priority="117" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:F15">
-    <cfRule type="cellIs" dxfId="153" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="75" operator="greaterThan">
       <formula>0.685</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="152" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="160" priority="110" operator="greaterThan">
       <formula>0.6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G9 G13:G15">
-    <cfRule type="cellIs" dxfId="151" priority="103" operator="greaterThan">
+  <conditionalFormatting sqref="G6:G9 G13:G15 AZ6:AZ11">
+    <cfRule type="cellIs" dxfId="159" priority="112" operator="greaterThan">
+      <formula>0.86</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="116" operator="greaterThan">
       <formula>0.85</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="99" operator="greaterThan">
-      <formula>0.86</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H15 H6:H9">
-    <cfRule type="cellIs" dxfId="149" priority="102" operator="lessThan">
+    <cfRule type="cellIs" dxfId="157" priority="115" operator="lessThan">
       <formula>0.195</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H15">
-    <cfRule type="cellIs" dxfId="148" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="156" priority="73" operator="lessThan">
       <formula>0.24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="60" operator="lessThan">
+    <cfRule type="cellIs" dxfId="155" priority="74" operator="lessThan">
       <formula>0.24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="146" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="108" operator="greaterThan">
       <formula>0.22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="109" operator="greaterThan">
       <formula>0.227</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I15">
-    <cfRule type="cellIs" dxfId="144" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="72" operator="greaterThan">
       <formula>0.7605</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="143" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="107" operator="greaterThan">
       <formula>0.77</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:J9 J13:J15">
-    <cfRule type="cellIs" dxfId="142" priority="100" operator="greaterThan">
+  <conditionalFormatting sqref="J6:J9 J13:J15 BC6:BC11">
+    <cfRule type="cellIs" dxfId="150" priority="113" operator="greaterThan">
       <formula>0.68</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:J15">
-    <cfRule type="cellIs" dxfId="141" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="71" operator="greaterThan">
       <formula>0.616</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="140" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="106" operator="greaterThan">
       <formula>0.63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:N9 N13:N15">
-    <cfRule type="cellIs" dxfId="139" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="105" operator="greaterThan">
       <formula>0.92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13:N15">
-    <cfRule type="cellIs" dxfId="138" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="46" operator="greaterThan">
       <formula>0.8925</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="137" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="93" operator="greaterThan">
       <formula>0.89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6:O9">
-    <cfRule type="cellIs" dxfId="136" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="69" operator="greaterThan">
       <formula>0.604</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13:O15">
-    <cfRule type="cellIs" dxfId="135" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="70" operator="greaterThan">
       <formula>0.7815</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P6:P9">
+    <cfRule type="cellIs" dxfId="142" priority="15" operator="greaterThan">
+      <formula>0.764</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P13:P15">
+    <cfRule type="cellIs" dxfId="141" priority="14" operator="greaterThan">
+      <formula>0.7095</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q6:Q9">
-    <cfRule type="cellIs" dxfId="134" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="140" priority="68" operator="lessThan">
       <formula>0.485</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13:Q15">
-    <cfRule type="cellIs" dxfId="133" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="139" priority="67" operator="lessThan">
       <formula>0.32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6:R9">
-    <cfRule type="cellIs" dxfId="132" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="66" operator="greaterThan">
       <formula>0.589</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R13:R15">
-    <cfRule type="cellIs" dxfId="131" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="65" operator="greaterThan">
       <formula>0.7385</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="130" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="95" operator="greaterThan">
       <formula>0.77</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S9">
-    <cfRule type="cellIs" dxfId="129" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="64" operator="greaterThan">
       <formula>0.447</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13:S15">
-    <cfRule type="cellIs" dxfId="128" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="63" operator="greaterThan">
       <formula>0.5875</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="cellIs" dxfId="127" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="94" operator="greaterThan">
       <formula>0.63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W6:W7 W13:W14">
-    <cfRule type="cellIs" dxfId="126" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="92" operator="greaterThan">
       <formula>0.93</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W13:W14">
-    <cfRule type="cellIs" dxfId="125" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="81" operator="greaterThan">
       <formula>0.8715</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6:X7 AA6:AA7 X13:X14 AA13:AA14">
-    <cfRule type="cellIs" dxfId="124" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="91" operator="greaterThan">
       <formula>0.768</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13:X14">
-    <cfRule type="cellIs" dxfId="123" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="80" operator="greaterThan">
       <formula>0.667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6:Y7 Y13:Y14">
-    <cfRule type="cellIs" dxfId="122" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="88" operator="greaterThan">
       <formula>0.794</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z6:Z7 Z13:Z14">
-    <cfRule type="cellIs" dxfId="121" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="90" operator="lessThan">
       <formula>0.255</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA13:AA14">
-    <cfRule type="cellIs" dxfId="120" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="79" operator="greaterThan">
       <formula>0.7355</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6:AB7 AB13:AB14">
-    <cfRule type="cellIs" dxfId="119" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="89" operator="greaterThan">
       <formula>0.61</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB13:AB14">
-    <cfRule type="cellIs" dxfId="118" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="78" operator="greaterThan">
       <formula>0.5845</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF6:AF9 AF13:AF15">
-    <cfRule type="cellIs" dxfId="117" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="62" operator="greaterThan">
       <formula>0.92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF13:AF15">
-    <cfRule type="cellIs" dxfId="116" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="47" operator="greaterThan">
       <formula>0.89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF6:AG9">
-    <cfRule type="cellIs" dxfId="115" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="44" operator="greaterThan">
       <formula>0.1325</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF13:AK15">
-    <cfRule type="cellIs" dxfId="114" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="37" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG6:AG9">
-    <cfRule type="cellIs" dxfId="113" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="56" operator="greaterThan">
       <formula>0.604</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG13:AG15">
-    <cfRule type="cellIs" dxfId="112" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="57" operator="greaterThan">
       <formula>0.7815</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH6:AH9">
-    <cfRule type="cellIs" dxfId="111" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH6:AH15">
-    <cfRule type="cellIs" dxfId="110" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6:AI9">
-    <cfRule type="cellIs" dxfId="108" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="40" operator="lessThan">
       <formula>0.81</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI13:AI15">
-    <cfRule type="cellIs" dxfId="107" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="54" operator="lessThan">
       <formula>0.32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ6:AJ9">
-    <cfRule type="cellIs" dxfId="106" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="39" operator="greaterThan">
       <formula>0.2205</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ13:AJ15">
-    <cfRule type="cellIs" dxfId="105" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="49" operator="greaterThan">
       <formula>0.77</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="52" operator="greaterThan">
       <formula>0.7385</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK6:AK9">
-    <cfRule type="cellIs" dxfId="103" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="38" operator="greaterThan">
+      <formula>0.1325</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="51" operator="greaterThan">
       <formula>0.447</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="25" operator="greaterThan">
-      <formula>0.1325</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK13:AK15">
-    <cfRule type="cellIs" dxfId="101" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="48" operator="greaterThan">
+      <formula>0.63</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="50" operator="greaterThan">
       <formula>0.5875</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="35" operator="greaterThan">
-      <formula>0.63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO6:AO9 AO13:AO15">
-    <cfRule type="cellIs" dxfId="99" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="34" operator="greaterThan">
       <formula>0.92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO13:AO15">
-    <cfRule type="cellIs" dxfId="98" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="25" operator="greaterThan">
       <formula>0.89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO6:AP9">
-    <cfRule type="cellIs" dxfId="97" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="24" operator="greaterThan">
       <formula>0.1325</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO13:AT15">
-    <cfRule type="cellIs" dxfId="96" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP6:AP9">
-    <cfRule type="cellIs" dxfId="95" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="32" operator="greaterThan">
       <formula>0.604</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP13:AP15">
-    <cfRule type="cellIs" dxfId="94" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="33" operator="greaterThan">
       <formula>0.7815</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ6:AQ9">
-    <cfRule type="cellIs" dxfId="93" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ6:AQ15">
-    <cfRule type="cellIs" dxfId="92" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR6:AR9">
-    <cfRule type="cellIs" dxfId="90" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="22" operator="lessThan">
       <formula>0.81</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR13:AR15">
-    <cfRule type="cellIs" dxfId="89" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="31" operator="lessThan">
       <formula>0.32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS6:AS9">
-    <cfRule type="cellIs" dxfId="88" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="21" operator="greaterThan">
       <formula>0.2205</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS13:AS15">
-    <cfRule type="cellIs" dxfId="87" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="27" operator="greaterThan">
       <formula>0.77</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="30" operator="greaterThan">
       <formula>0.7385</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT6:AT9">
-    <cfRule type="cellIs" dxfId="85" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="20" operator="greaterThan">
       <formula>0.1325</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="29" operator="greaterThan">
       <formula>0.447</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT13:AT15">
-    <cfRule type="cellIs" dxfId="83" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="26" operator="greaterThan">
+      <formula>0.63</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="28" operator="greaterThan">
       <formula>0.5875</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="13" operator="greaterThan">
-      <formula>0.63</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX6:AX11">
+    <cfRule type="cellIs" dxfId="87" priority="6" operator="greaterThan">
+      <formula>0.935</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G9">
-    <cfRule type="cellIs" dxfId="81" priority="3" operator="greaterThan">
-      <formula>0.8135</formula>
+  <conditionalFormatting sqref="AZ6:AZ11">
+    <cfRule type="cellIs" dxfId="86" priority="5" operator="greaterThan">
+      <formula>0.89</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P6:P9">
-    <cfRule type="cellIs" dxfId="80" priority="2" operator="greaterThan">
-      <formula>0.764</formula>
+  <conditionalFormatting sqref="BA6:BA11">
+    <cfRule type="cellIs" dxfId="85" priority="3" operator="lessThan">
+      <formula>0.22</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P13:P15">
+  <conditionalFormatting sqref="BB6:BB11">
+    <cfRule type="cellIs" dxfId="84" priority="2" operator="greaterThan">
+      <formula>0.78</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC6:BC11">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>0.7095</formula>
+      <formula>0.65</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added result images and updated results
</commit_message>
<xml_diff>
--- a/Models/Metrics.xlsx
+++ b/Models/Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\Desktop\Università\Tesi magistrale\FedMix\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D77E161-8572-4377-8BF7-E0305C754274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7B11EA-4FF8-4B8D-A673-19358A26E551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9681,7 +9681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844EB822-0A82-415C-A215-29BF00E2AD44}">
   <dimension ref="D4:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="J19" sqref="J19:J22"/>
     </sheetView>
   </sheetViews>

</xml_diff>